<commit_message>
adding last crud operations
</commit_message>
<xml_diff>
--- a/NWU Tech Trends Telemetry Portal User Acceptance Testing_/NWU Tech Trends Data.xlsx
+++ b/NWU Tech Trends Telemetry Portal User Acceptance Testing_/NWU Tech Trends Data.xlsx
@@ -1,36 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brand\OneDrive\Desktop\JM Repo\JM Work Repo\NWU\Modules\2024 CMPG323\Project 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\UiPath\NWU Tech Trends Telemetry Portal User Acceptance Testing_\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B432EAD3-C6FE-4098-AA29-885124F46384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E1D197-0B73-45AB-98E9-F63C558B4936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CD795CCD-582F-4BD0-AF39-75E63E90AABB}"/>
+    <workbookView xWindow="1770" yWindow="3780" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{CD795CCD-582F-4BD0-AF39-75E63E90AABB}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
     <sheet name="Projects" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1325,7 +1314,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,6 +1354,9 @@
       <c r="D2" s="2">
         <v>44941</v>
       </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1379,6 +1371,9 @@
       <c r="D3" s="2">
         <v>44942</v>
       </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1393,6 +1388,9 @@
       <c r="D4" s="2">
         <v>44943</v>
       </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1407,6 +1405,9 @@
       <c r="D5" s="2">
         <v>44944</v>
       </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1421,6 +1422,9 @@
       <c r="D6" s="2">
         <v>44945</v>
       </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1435,6 +1439,9 @@
       <c r="D7" s="2">
         <v>44946</v>
       </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1449,6 +1456,9 @@
       <c r="D8" s="2">
         <v>44947</v>
       </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1463,6 +1473,9 @@
       <c r="D9" s="2">
         <v>44948</v>
       </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1477,6 +1490,9 @@
       <c r="D10" s="2">
         <v>44949</v>
       </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1491,6 +1507,9 @@
       <c r="D11" s="2">
         <v>44950</v>
       </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1505,6 +1524,9 @@
       <c r="D12" s="2">
         <v>44951</v>
       </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1519,6 +1541,9 @@
       <c r="D13" s="2">
         <v>44952</v>
       </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1533,6 +1558,9 @@
       <c r="D14" s="2">
         <v>44953</v>
       </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1547,6 +1575,9 @@
       <c r="D15" s="2">
         <v>44954</v>
       </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1561,8 +1592,11 @@
       <c r="D16" s="2">
         <v>44955</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>120</v>
       </c>
@@ -1575,8 +1609,11 @@
       <c r="D17" s="2">
         <v>44956</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>121</v>
       </c>
@@ -1589,8 +1626,11 @@
       <c r="D18" s="2">
         <v>44957</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>122</v>
       </c>
@@ -1603,8 +1643,11 @@
       <c r="D19" s="2">
         <v>44958</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>123</v>
       </c>
@@ -1617,8 +1660,11 @@
       <c r="D20" s="2">
         <v>44959</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>124</v>
       </c>
@@ -1631,8 +1677,11 @@
       <c r="D21" s="2">
         <v>44960</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>125</v>
       </c>
@@ -1645,8 +1694,11 @@
       <c r="D22" s="2">
         <v>44961</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>126</v>
       </c>
@@ -1659,8 +1711,11 @@
       <c r="D23" s="2">
         <v>44962</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>127</v>
       </c>
@@ -1673,8 +1728,11 @@
       <c r="D24" s="2">
         <v>44963</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>128</v>
       </c>
@@ -1687,8 +1745,11 @@
       <c r="D25" s="2">
         <v>44964</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>129</v>
       </c>
@@ -1701,8 +1762,11 @@
       <c r="D26" s="2">
         <v>44965</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>130</v>
       </c>
@@ -1715,8 +1779,11 @@
       <c r="D27" s="2">
         <v>44966</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -1729,8 +1796,11 @@
       <c r="D28" s="2">
         <v>44967</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>132</v>
       </c>
@@ -1743,8 +1813,11 @@
       <c r="D29" s="2">
         <v>44968</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>133</v>
       </c>
@@ -1757,8 +1830,11 @@
       <c r="D30" s="2">
         <v>44969</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>134</v>
       </c>
@@ -1771,8 +1847,11 @@
       <c r="D31" s="2">
         <v>44970</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>135</v>
       </c>
@@ -1785,8 +1864,11 @@
       <c r="D32" s="2">
         <v>44971</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>136</v>
       </c>
@@ -1799,8 +1881,11 @@
       <c r="D33" s="2">
         <v>44972</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>137</v>
       </c>
@@ -1813,8 +1898,11 @@
       <c r="D34" s="2">
         <v>44973</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>138</v>
       </c>
@@ -1827,8 +1915,11 @@
       <c r="D35" s="2">
         <v>44974</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>139</v>
       </c>
@@ -1841,8 +1932,11 @@
       <c r="D36" s="2">
         <v>44975</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>140</v>
       </c>
@@ -1855,8 +1949,11 @@
       <c r="D37" s="2">
         <v>44976</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>141</v>
       </c>
@@ -1869,8 +1966,11 @@
       <c r="D38" s="2">
         <v>44977</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>142</v>
       </c>
@@ -1883,8 +1983,11 @@
       <c r="D39" s="2">
         <v>44978</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>143</v>
       </c>
@@ -1897,8 +2000,11 @@
       <c r="D40" s="2">
         <v>44979</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>144</v>
       </c>
@@ -1911,8 +2017,11 @@
       <c r="D41" s="2">
         <v>44980</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>145</v>
       </c>
@@ -1925,8 +2034,11 @@
       <c r="D42" s="2">
         <v>44981</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>146</v>
       </c>
@@ -1939,8 +2051,11 @@
       <c r="D43" s="2">
         <v>44982</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>147</v>
       </c>
@@ -1953,8 +2068,11 @@
       <c r="D44" s="2">
         <v>44983</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>148</v>
       </c>
@@ -1967,8 +2085,11 @@
       <c r="D45" s="2">
         <v>44984</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>149</v>
       </c>
@@ -1981,8 +2102,11 @@
       <c r="D46" s="2">
         <v>44985</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>150</v>
       </c>
@@ -1995,8 +2119,11 @@
       <c r="D47" s="2">
         <v>44986</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>151</v>
       </c>
@@ -2009,8 +2136,11 @@
       <c r="D48" s="2">
         <v>44987</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>152</v>
       </c>
@@ -2023,8 +2153,11 @@
       <c r="D49" s="2">
         <v>44988</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>153</v>
       </c>
@@ -2037,8 +2170,11 @@
       <c r="D50" s="2">
         <v>44989</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>154</v>
       </c>
@@ -2061,8 +2197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D331589-AA9D-4074-9BAA-5A515B94893D}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2116,6 +2252,9 @@
       <c r="F2" s="1" t="s">
         <v>105</v>
       </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -2136,6 +2275,9 @@
       <c r="F3" s="1" t="s">
         <v>106</v>
       </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -2156,6 +2298,9 @@
       <c r="F4" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -2176,6 +2321,9 @@
       <c r="F5" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -2196,6 +2344,9 @@
       <c r="F6" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2216,6 +2367,9 @@
       <c r="F7" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -2236,6 +2390,9 @@
       <c r="F8" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -2256,6 +2413,9 @@
       <c r="F9" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -2276,6 +2436,9 @@
       <c r="F10" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -2296,6 +2459,9 @@
       <c r="F11" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -2316,6 +2482,9 @@
       <c r="F12" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -2336,6 +2505,9 @@
       <c r="F13" s="1" t="s">
         <v>120</v>
       </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -2356,6 +2528,9 @@
       <c r="F14" s="1" t="s">
         <v>117</v>
       </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -2376,6 +2551,9 @@
       <c r="F15" s="1" t="s">
         <v>123</v>
       </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -2396,8 +2574,11 @@
       <c r="F16" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>208</v>
       </c>
@@ -2416,8 +2597,11 @@
       <c r="F17" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>211</v>
       </c>
@@ -2436,8 +2620,11 @@
       <c r="F18" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>214</v>
       </c>
@@ -2456,8 +2643,11 @@
       <c r="F19" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>217</v>
       </c>
@@ -2476,8 +2666,11 @@
       <c r="F20" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>220</v>
       </c>
@@ -2496,8 +2689,11 @@
       <c r="F21" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>223</v>
       </c>
@@ -2516,8 +2712,11 @@
       <c r="F22" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>226</v>
       </c>
@@ -2536,8 +2735,11 @@
       <c r="F23" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>229</v>
       </c>
@@ -2556,8 +2758,11 @@
       <c r="F24" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>232</v>
       </c>
@@ -2576,8 +2781,11 @@
       <c r="F25" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>235</v>
       </c>
@@ -2596,8 +2804,11 @@
       <c r="F26" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>238</v>
       </c>
@@ -2616,8 +2827,11 @@
       <c r="F27" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>241</v>
       </c>
@@ -2636,8 +2850,11 @@
       <c r="F28" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>244</v>
       </c>
@@ -2656,8 +2873,11 @@
       <c r="F29" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>247</v>
       </c>
@@ -2676,8 +2896,11 @@
       <c r="F30" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>250</v>
       </c>
@@ -2696,8 +2919,11 @@
       <c r="F31" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>253</v>
       </c>
@@ -2716,8 +2942,11 @@
       <c r="F32" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>256</v>
       </c>
@@ -2736,8 +2965,11 @@
       <c r="F33" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>259</v>
       </c>
@@ -2756,8 +2988,11 @@
       <c r="F34" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>262</v>
       </c>
@@ -2776,8 +3011,11 @@
       <c r="F35" s="1" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>265</v>
       </c>
@@ -2796,8 +3034,11 @@
       <c r="F36" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>268</v>
       </c>
@@ -2816,8 +3057,11 @@
       <c r="F37" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>271</v>
       </c>
@@ -2836,8 +3080,11 @@
       <c r="F38" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>274</v>
       </c>
@@ -2856,8 +3103,11 @@
       <c r="F39" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>277</v>
       </c>
@@ -2876,8 +3126,11 @@
       <c r="F40" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>280</v>
       </c>
@@ -2896,8 +3149,11 @@
       <c r="F41" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>283</v>
       </c>
@@ -2916,8 +3172,11 @@
       <c r="F42" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>286</v>
       </c>
@@ -2936,8 +3195,11 @@
       <c r="F43" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>289</v>
       </c>
@@ -2956,8 +3218,11 @@
       <c r="F44" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>292</v>
       </c>
@@ -2976,8 +3241,11 @@
       <c r="F45" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>295</v>
       </c>
@@ -2995,6 +3263,9 @@
       </c>
       <c r="F46" s="1" t="s">
         <v>117</v>
+      </c>
+      <c r="G46" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>